<commit_message>
Added partial constraints example
</commit_message>
<xml_diff>
--- a/examples/island (partial mga)/simulation_times.xlsx
+++ b/examples/island (partial mga)/simulation_times.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://aarhusuniversitet-my.sharepoint.com/personal/au592788_uni_au_dk/Documents/Dokumenter/Github/PyMGA_LBN/examples/island (partial mga)/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="103" documentId="11_AD4D1D646341095ACB7000D8CD94D484683EDF25" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A1B8D01F-D838-4AA0-B7FF-70CCFB20720F}"/>
+  <xr:revisionPtr revIDLastSave="107" documentId="11_AD4D1D646341095ACB7000D8CD94D484683EDF25" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{989CDEA9-2462-41FA-B307-EA6FE95B244A}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -94,10 +94,10 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -382,10 +382,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:W23"/>
+  <dimension ref="B2:W25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R5" sqref="R5"/>
+      <selection activeCell="L25" sqref="L25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -405,13 +405,13 @@
       <c r="H2" s="3"/>
     </row>
     <row r="3" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
     </row>
     <row r="4" spans="2:23" x14ac:dyDescent="0.3">
       <c r="D4">
@@ -431,7 +431,7 @@
       </c>
     </row>
     <row r="5" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C5">
@@ -448,7 +448,7 @@
       </c>
     </row>
     <row r="6" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B6" s="2"/>
+      <c r="B6" s="1"/>
       <c r="C6">
         <v>4</v>
       </c>
@@ -457,7 +457,7 @@
       </c>
     </row>
     <row r="7" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B7" s="2"/>
+      <c r="B7" s="1"/>
       <c r="C7">
         <v>5</v>
       </c>
@@ -469,7 +469,7 @@
       </c>
     </row>
     <row r="8" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B8" s="2"/>
+      <c r="B8" s="1"/>
       <c r="C8">
         <v>6</v>
       </c>
@@ -484,19 +484,19 @@
       </c>
     </row>
     <row r="9" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B9" s="2"/>
+      <c r="B9" s="1"/>
       <c r="C9">
         <v>7</v>
       </c>
     </row>
     <row r="10" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B10" s="2"/>
+      <c r="B10" s="1"/>
       <c r="C10">
         <v>8</v>
       </c>
     </row>
     <row r="11" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B11" s="2"/>
+      <c r="B11" s="1"/>
       <c r="C11">
         <v>9</v>
       </c>
@@ -514,13 +514,13 @@
       <c r="H14" s="3"/>
     </row>
     <row r="15" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="D15" s="1" t="s">
+      <c r="D15" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
     </row>
     <row r="16" spans="2:23" x14ac:dyDescent="0.3">
       <c r="D16">
@@ -558,7 +558,7 @@
       </c>
     </row>
     <row r="17" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C17">
@@ -572,19 +572,19 @@
       </c>
     </row>
     <row r="18" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B18" s="2"/>
+      <c r="B18" s="1"/>
       <c r="C18">
         <v>4</v>
       </c>
     </row>
     <row r="19" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B19" s="2"/>
+      <c r="B19" s="1"/>
       <c r="C19">
         <v>5</v>
       </c>
     </row>
     <row r="20" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B20" s="2"/>
+      <c r="B20" s="1"/>
       <c r="C20">
         <v>6</v>
       </c>
@@ -593,19 +593,19 @@
       </c>
     </row>
     <row r="21" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B21" s="2"/>
+      <c r="B21" s="1"/>
       <c r="C21">
         <v>7</v>
       </c>
     </row>
     <row r="22" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B22" s="2"/>
+      <c r="B22" s="1"/>
       <c r="C22">
         <v>8</v>
       </c>
     </row>
     <row r="23" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B23" s="2"/>
+      <c r="B23" s="1"/>
       <c r="C23">
         <v>9</v>
       </c>
@@ -634,14 +634,32 @@
         <v>2241</v>
       </c>
     </row>
+    <row r="25" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="G25">
+        <f t="shared" ref="G25:I25" si="0">G23/3600</f>
+        <v>0.11388888888888889</v>
+      </c>
+      <c r="H25">
+        <f t="shared" si="0"/>
+        <v>0.20166666666666666</v>
+      </c>
+      <c r="I25">
+        <f t="shared" si="0"/>
+        <v>0.5805555555555556</v>
+      </c>
+      <c r="J25">
+        <f>J23/3600</f>
+        <v>2.0038888888888891</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="D2:H2"/>
     <mergeCell ref="B5:B11"/>
     <mergeCell ref="D3:H3"/>
     <mergeCell ref="D15:H15"/>
     <mergeCell ref="B17:B23"/>
     <mergeCell ref="D14:H14"/>
-    <mergeCell ref="D2:H2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>